<commit_message>
First light UCC results.
</commit_message>
<xml_diff>
--- a/data/zaf_2013_ecc.xlsx
+++ b/data/zaf_2013_ecc.xlsx
@@ -10,22 +10,22 @@
     <sheet name="ZAF_2013_X" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="R_ZAF_2013_E">'ZAF_2013_E'!$B$157:$AO$183</definedName>
-    <definedName name="U_ZAF_2013_E">'ZAF_2013_E'!$AS$90:$BK$129</definedName>
-    <definedName name="V_ZAF_2013_E">'ZAF_2013_E'!$B$134:$AO$152</definedName>
-    <definedName name="Y_ZAF_2013_E">'ZAF_2013_E'!$BO$90:$DF$129</definedName>
-    <definedName name="r_eiou_ZAF_2013_E">'ZAF_2013_E'!$BO$2:$CG$41</definedName>
-    <definedName name="U_eiou_ZAF_2013_E">'ZAF_2013_E'!$AS$2:$BK$41</definedName>
-    <definedName name="U_feed_ZAF_2013_E">'ZAF_2013_E'!$AS$46:$BK$85</definedName>
-    <definedName name="S_units_ZAF_2013_E">'ZAF_2013_E'!$B$2:$B$45</definedName>
-    <definedName name="R_ZAF_2013_X">'ZAF_2013_X'!$B$157:$AO$183</definedName>
-    <definedName name="U_ZAF_2013_X">'ZAF_2013_X'!$AS$90:$BK$129</definedName>
-    <definedName name="V_ZAF_2013_X">'ZAF_2013_X'!$B$134:$AO$152</definedName>
-    <definedName name="Y_ZAF_2013_X">'ZAF_2013_X'!$BO$90:$DF$129</definedName>
-    <definedName name="r_eiou_ZAF_2013_X">'ZAF_2013_X'!$BO$2:$CG$41</definedName>
-    <definedName name="U_eiou_ZAF_2013_X">'ZAF_2013_X'!$AS$2:$BK$41</definedName>
-    <definedName name="U_feed_ZAF_2013_X">'ZAF_2013_X'!$AS$46:$BK$85</definedName>
-    <definedName name="S_units_ZAF_2013_X">'ZAF_2013_X'!$B$2:$B$45</definedName>
+    <definedName name="R__ZAF_2013_E">'ZAF_2013_E'!$A$156:$AO$183</definedName>
+    <definedName name="U__ZAF_2013_E">'ZAF_2013_E'!$AR$89:$BK$129</definedName>
+    <definedName name="V__ZAF_2013_E">'ZAF_2013_E'!$A$133:$AO$152</definedName>
+    <definedName name="Y__ZAF_2013_E">'ZAF_2013_E'!$BN$89:$DF$129</definedName>
+    <definedName name="r_EIOU__ZAF_2013_E">'ZAF_2013_E'!$BN$1:$CG$41</definedName>
+    <definedName name="U_EIOU__ZAF_2013_E">'ZAF_2013_E'!$AR$1:$BK$41</definedName>
+    <definedName name="U_feed__ZAF_2013_E">'ZAF_2013_E'!$AR$45:$BK$85</definedName>
+    <definedName name="S_units__ZAF_2013_E">'ZAF_2013_E'!$A$1:$B$45</definedName>
+    <definedName name="R__ZAF_2013_X">'ZAF_2013_X'!$A$156:$AO$183</definedName>
+    <definedName name="U__ZAF_2013_X">'ZAF_2013_X'!$AR$89:$BK$129</definedName>
+    <definedName name="V__ZAF_2013_X">'ZAF_2013_X'!$A$133:$AO$152</definedName>
+    <definedName name="Y__ZAF_2013_X">'ZAF_2013_X'!$BN$89:$DF$129</definedName>
+    <definedName name="r_EIOU__ZAF_2013_X">'ZAF_2013_X'!$BN$1:$CG$41</definedName>
+    <definedName name="U_EIOU__ZAF_2013_X">'ZAF_2013_X'!$AR$1:$BK$41</definedName>
+    <definedName name="U_feed__ZAF_2013_X">'ZAF_2013_X'!$AR$45:$BK$85</definedName>
+    <definedName name="S_units__ZAF_2013_X">'ZAF_2013_X'!$A$1:$B$45</definedName>
   </definedNames>
 </workbook>
 </file>
@@ -435,10 +435,10 @@
     <t xml:space="preserve">Y</t>
   </si>
   <si>
-    <t xml:space="preserve">r_eiou</t>
+    <t xml:space="preserve">r_EIOU</t>
   </si>
   <si>
-    <t xml:space="preserve">U_eiou</t>
+    <t xml:space="preserve">U_EIOU</t>
   </si>
   <si>
     <t xml:space="preserve">U_feed</t>

</xml_diff>